<commit_message>
Update 20240619_Data summary_Sumera Perveen_Aggregation and PicoGreen_CNP17.xlsx
</commit_message>
<xml_diff>
--- a/Covalent raw data/20240619_Data summary_Sumera Perveen_Aggregation and PicoGreen_CNP17.xlsx
+++ b/Covalent raw data/20240619_Data summary_Sumera Perveen_Aggregation and PicoGreen_CNP17.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uccaris_ucl_ac_uk/Documents/DENV project/Datasets/Enamine covalent/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveuclac-my.sharepoint.com/personal/uccaris_ucl_ac_uk/Documents/GitHub/CNP17-DENVRdrp-EnamineCovalent/Covalent raw data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="26" documentId="8_{98001144-0200-4950-BF07-1F008870CA8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{192CB620-4CC8-4833-A563-77B51B5C6B18}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{230FC801-4F24-42AA-B300-740ECDECD33A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{230FC801-4F24-42AA-B300-740ECDECD33A}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary assays" sheetId="3" r:id="rId1"/>
@@ -218,10 +218,7 @@
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -235,6 +232,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1376,7 +1376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADCD8F56-EDC3-4366-A1F8-9E6FD17646F8}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
@@ -1389,290 +1389,290 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>584</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1101</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1040</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>100</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>100</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>1544</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>638</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>1060</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>100</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>100</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>2723</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1471</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>1657</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="6">
         <v>65</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="6">
         <v>85</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>3021</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>656</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>715</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>95</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>100</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>594</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>636</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>586</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>100</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="7">
         <v>100</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="7">
         <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>3272</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2911</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>1990</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E8" s="6">
         <v>40</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="6">
         <v>40</v>
       </c>
-      <c r="G8" s="7">
+      <c r="G8" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>3998</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>3652</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>2449</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <v>35</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="6">
         <v>38</v>
       </c>
-      <c r="G9" s="7">
+      <c r="G9" s="6">
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>2867</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>2472</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>2972</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E10" s="6">
         <v>45</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="6">
         <v>50</v>
       </c>
-      <c r="G10" s="7">
+      <c r="G10" s="6">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B11" s="5">
         <v>285270</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>9346</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>6353</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E11" s="6">
         <v>15</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>25</v>
       </c>
-      <c r="G11" s="7">
+      <c r="G11" s="6">
         <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="5">
         <v>2649</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="5">
         <v>1529</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>1658</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="6">
         <v>40</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="6">
         <v>63</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>736</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>1164</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>1195</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>100</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>100</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>95</v>
       </c>
     </row>
@@ -1696,8 +1696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8DEBBF-EBF4-4422-8581-BD4CDFDBE350}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,34 +1707,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>